<commit_message>
Update planning, code and purchase file(motor)
</commit_message>
<xml_diff>
--- a/Components.xlsx
+++ b/Components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://technionchina-my.sharepoint.com/personal/zeng12875_gtiit_edu_cn/Documents/学习/大三下/Project in Design for Manufacturing_/Project-in-Design-2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34F91A02-CFB6-B747-8A67-E6763F72E0CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="8_{34F91A02-CFB6-B747-8A67-E6763F72E0CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7B7F620-E624-1E46-98D3-04102643CC67}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="17160" windowHeight="21600" xr2:uid="{AC99C891-B10B-1842-81EE-FD08F50E8A2C}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="29660" windowHeight="21580" xr2:uid="{AC99C891-B10B-1842-81EE-FD08F50E8A2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,36 +36,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Components</t>
   </si>
   <si>
-    <t xml:space="preserve">Basement </t>
-  </si>
-  <si>
-    <t>Wheels</t>
-  </si>
-  <si>
-    <t>Tower</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Robot Arm </t>
-  </si>
-  <si>
-    <t>Container</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telescopic </t>
-  </si>
-  <si>
     <t>Bearing</t>
   </si>
   <si>
-    <t>Belt</t>
-  </si>
-  <si>
     <t xml:space="preserve">Movement </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Servo Motor </t>
+  </si>
+  <si>
+    <t>Gear</t>
+  </si>
+  <si>
+    <t>blades</t>
+  </si>
+  <si>
+    <t>Housing</t>
+  </si>
+  <si>
+    <t>Tube</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connection </t>
+  </si>
+  <si>
+    <t>Shaft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scissor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">End effector  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elevator </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beam </t>
+  </si>
+  <si>
+    <t>Power Screw</t>
+  </si>
+  <si>
+    <t>Motor</t>
+  </si>
+  <si>
+    <t>Turn Table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connetion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table </t>
   </si>
 </sst>
 </file>
@@ -101,8 +134,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,58 +453,188 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B792334-60EE-1D4A-95E7-04155ED96E9A}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="222" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="213" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
         <v>8</v>
       </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>